<commit_message>
Added wood and propane to excel spreadsheet
</commit_message>
<xml_diff>
--- a/data/Services.xlsx
+++ b/data/Services.xlsx
@@ -22,6 +22,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Alan</author>
+    <author>dustin</author>
   </authors>
   <commentList>
     <comment ref="A3" authorId="0">
@@ -105,12 +106,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="C15" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>dustin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Assume 50% spruce and 50% birch</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>lbs</t>
   </si>
@@ -216,6 +241,21 @@
       <t>(make sure "Service Type" header row starts on Row 3)</t>
     </r>
   </si>
+  <si>
+    <t>Wood</t>
+  </si>
+  <si>
+    <t>cords</t>
+  </si>
+  <si>
+    <t>wood</t>
+  </si>
+  <si>
+    <t>propane</t>
+  </si>
+  <si>
+    <t>Propane</t>
+  </si>
 </sst>
 </file>
 
@@ -225,7 +265,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -282,6 +322,19 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -644,7 +697,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -652,10 +705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -824,6 +877,35 @@
         <v>26</v>
       </c>
     </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15">
+        <f>(26200000+18100000)/2</f>
+        <v>22150000</v>
+      </c>
+      <c r="D15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <v>91800</v>
+      </c>
+      <c r="D16" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Added a method to Util object for Service Category info.
Maps standard fuel types like 'natural_gas' to their standard unit like 'CCF' and the Btus/unit for the fuel unit.
</commit_message>
<xml_diff>
--- a/data/Services.xlsx
+++ b/data/Services.xlsx
@@ -1,15 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tabb9\Documents\GitHub\fnsb-benchmark\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B808C7BC-1CD3-4612-B782-A95A807865F9}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Service Types" sheetId="1" r:id="rId1"/>
+    <sheet name="Service Categories" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,13 +26,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Alan</author>
-    <author>dustin</author>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -45,11 +51,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-All Service Types should be listed here.  For types that are Energy, include a separte row for each unit found in the input data and fill out Btus/Unit.  For non-energy types, units need not be listed, but Category should be filled out.</t>
+All Service Types that appear in the input utility record data set should be listed here.  For types that are Energy, include a separte row for each unit found in the input data and fill out Btus/Unit.  For non-energy types, units need not be listed, but Category should be filled out.  See the cell note in the Category column for the list of valid Categories.</t>
         </r>
       </text>
     </comment>
-    <comment ref="D3" authorId="0">
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -82,7 +88,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="0">
+    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -106,7 +112,91 @@
         </r>
       </text>
     </comment>
-    <comment ref="C15" authorId="1">
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Alan</author>
+    <author>Alan Mitchell</author>
+    <author>dustin</author>
+  </authors>
+  <commentList>
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{78086CE0-0CCA-4E19-9AE8-190F18AC5C00}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Alan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+These are the standard service type categories that are energy fuels.  Do *not* edit, add, or delete these categories.  You can only change the Unit types and the Btus/unit.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="1" shapeId="0" xr:uid="{D4E8A3A2-0D1A-447D-992C-587ECD6829B2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Alan Mitchell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+For the service category, this unit will be used when displaying physical consumption units.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C7" authorId="1" shapeId="0" xr:uid="{5AB48F94-EFD1-4CF3-867C-09B617D68AEA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Alan Mitchell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+FNSB is almost all #1 Oil, so use that for the category.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C9" authorId="2" shapeId="0" xr:uid="{105F493D-19F0-40D3-8BE2-02F01D7BAEB4}">
       <text>
         <r>
           <rPr>
@@ -135,7 +225,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="36">
   <si>
     <t>lbs</t>
   </si>
@@ -242,9 +332,6 @@
     </r>
   </si>
   <si>
-    <t>Wood</t>
-  </si>
-  <si>
     <t>cords</t>
   </si>
   <si>
@@ -254,13 +341,16 @@
     <t>propane</t>
   </si>
   <si>
-    <t>Propane</t>
+    <t>Service Category</t>
+  </si>
+  <si>
+    <t>Information about standard fuel categories (header must start on Row 3)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -697,33 +787,33 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>28</v>
       </c>
@@ -737,7 +827,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>29</v>
       </c>
@@ -752,7 +842,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -766,7 +856,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -780,7 +870,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -794,7 +884,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -808,7 +898,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -822,7 +912,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -836,7 +926,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -850,7 +940,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -859,7 +949,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -868,7 +958,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -877,33 +967,120 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C91C7A99-8204-4F86-87AF-870BE3A561A0}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="9" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1">
+        <v>102000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1">
+        <v>3412</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1">
+        <v>135000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="B15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15">
-        <f>(26200000+18100000)/2</f>
-        <v>22150000</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="C9" s="1">
+        <f>(23600000+18100000)/2</f>
+        <v>20850000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="B10" t="s">
         <v>4</v>
       </c>
-      <c r="C16">
+      <c r="C10" s="1">
         <v>91800</v>
-      </c>
-      <c r="D16" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Used service category info to calculate physical consumption units.
</commit_message>
<xml_diff>
--- a/data/Services.xlsx
+++ b/data/Services.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tabb9\Documents\GitHub\fnsb-benchmark\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B808C7BC-1CD3-4612-B782-A95A807865F9}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6EA39E31-E476-4CE3-BB5F-024305B389B0}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Service Types" sheetId="1" r:id="rId1"/>
@@ -332,9 +332,6 @@
     </r>
   </si>
   <si>
-    <t>cords</t>
-  </si>
-  <si>
     <t>wood</t>
   </si>
   <si>
@@ -345,6 +342,9 @@
   </si>
   <si>
     <t>Information about standard fuel categories (header must start on Row 3)</t>
+  </si>
+  <si>
+    <t>Cords</t>
   </si>
 </sst>
 </file>
@@ -797,7 +797,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -978,8 +978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C91C7A99-8204-4F86-87AF-870BE3A561A0}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -991,12 +991,12 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>13</v>
@@ -1062,10 +1062,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C9" s="1">
         <f>(23600000+18100000)/2</f>
@@ -1074,7 +1074,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
         <v>4</v>

</xml_diff>